<commit_message>
updated auto-generation of pages
</commit_message>
<xml_diff>
--- a/assets/LadenburgConsensuStatements.xlsx
+++ b/assets/LadenburgConsensuStatements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zauner/Documents/Arbeit/12-TUM/_Misc/2024-04_Ladenburg_Roundtable/LCS/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009469B6-A562-CE4F-9F7C-5CEDFAEE0763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DBCD22-7381-3D4C-85D5-BAA11D467BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="760" windowWidth="16740" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6220" yWindow="760" windowWidth="28340" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="4" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Individual differences in light sensitivity are influenced by factors such as age, genetics, and behavior.</t>
   </si>
   <si>
-    <t>Deutsche Übersetzung</t>
-  </si>
-  <si>
     <t>Es gibt erhebliche individuelle Unterschiede bei den physiologischen Reaktionen auf Licht</t>
   </si>
   <si>
@@ -718,6 +715,9 @@
   </si>
   <si>
     <t>Kontextinformation</t>
+  </si>
+  <si>
+    <t>German</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F22FC8-674F-B042-9987-EED3C133DD60}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -1617,7 +1617,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1626,18 +1626,18 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1646,18 +1646,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1666,18 +1666,18 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="F3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1686,18 +1686,18 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1706,38 +1706,38 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1746,18 +1746,18 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1766,18 +1766,18 @@
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1786,18 +1786,18 @@
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1806,18 +1806,18 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1826,38 +1826,38 @@
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1866,18 +1866,18 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1886,18 +1886,18 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1906,18 +1906,18 @@
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1926,18 +1926,18 @@
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1946,18 +1946,18 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="340" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1969,15 +1969,15 @@
         <v>28</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1989,15 +1989,15 @@
         <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -2006,18 +2006,18 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -2026,18 +2026,18 @@
         <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="404" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -2052,12 +2052,12 @@
         <v>32</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -2066,18 +2066,18 @@
         <v>23</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -2086,18 +2086,18 @@
         <v>24</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2106,18 +2106,18 @@
         <v>25</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="F25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -2126,18 +2126,18 @@
         <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="F26" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -2149,10 +2149,10 @@
         <v>30</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2178,464 +2178,464 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="163" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="181.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="187" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B27" s="1">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2647,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0227B8-6517-D949-81F0-BC1F8DC37DAA}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
@@ -2659,50 +2659,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>34</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="119" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="84" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="88" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="147" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>